<commit_message>
add task list to tooltip for stories in view page
</commit_message>
<xml_diff>
--- a/data/2025_goals.xlsx
+++ b/data/2025_goals.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tferenc/ebis/task_management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tferenc/ebis/task_management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A9BC072-2761-AB48-92E6-6DE8CB86F90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449ACB7A-697E-204D-9C2E-4EEA87153DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1640" windowWidth="38400" windowHeight="19420" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
+    <workbookView xWindow="38380" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaulation 2024" sheetId="2" r:id="rId1"/>
+    <sheet name="goals 2025" sheetId="1" r:id="rId2"/>
+    <sheet name="Objectives" sheetId="3" r:id="rId3"/>
+    <sheet name="PI planning" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="152">
   <si>
     <t>dbt</t>
   </si>
@@ -137,17 +140,377 @@
     <t>France trip</t>
   </si>
   <si>
+    <t>objectives:</t>
+  </si>
+  <si>
+    <t>Nose surgery</t>
+  </si>
+  <si>
+    <t>objectives</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>complitation_date</t>
+  </si>
+  <si>
+    <t>acceptance_criteria</t>
+  </si>
+  <si>
+    <t>mieć wieksza moc</t>
+  </si>
+  <si>
+    <t>nauczyc się jezdzic na kole</t>
+  </si>
+  <si>
+    <t>fill comfortable with sex</t>
+  </si>
+  <si>
     <t>Sex improvment</t>
+  </si>
+  <si>
+    <t>Go to mountin for weekend without kids</t>
+  </si>
+  <si>
+    <t>Go somewhere with kids for a weekend</t>
+  </si>
+  <si>
+    <t>Read 4 books</t>
+  </si>
+  <si>
+    <t>Gain 1 certification</t>
+  </si>
+  <si>
+    <t>Service improvment</t>
+  </si>
+  <si>
+    <t>Attend to one data conference</t>
+  </si>
+  <si>
+    <t>ems</t>
+  </si>
+  <si>
+    <t>wycieczka</t>
+  </si>
+  <si>
+    <t>dbanie o stopy</t>
+  </si>
+  <si>
+    <t>dbanie o ubranie</t>
+  </si>
+  <si>
+    <t>operacja na krzywa przegrode nosa</t>
+  </si>
+  <si>
+    <t>Sport/Health</t>
+  </si>
+  <si>
+    <t>jazda na rowerze w peletonie</t>
+  </si>
+  <si>
+    <t>Personal Development</t>
+  </si>
+  <si>
+    <t>dbt certification</t>
+  </si>
+  <si>
+    <t>power bi basics</t>
+  </si>
+  <si>
+    <t>aws basics</t>
+  </si>
+  <si>
+    <t>air flow</t>
+  </si>
+  <si>
+    <t>python streamlit pandas</t>
+  </si>
+  <si>
+    <t>snowflake/data warehousing</t>
+  </si>
+  <si>
+    <t>Entertaiment</t>
+  </si>
+  <si>
+    <t>spotykanie z ludzmi</t>
+  </si>
+  <si>
+    <t>dolaczenie do jakiejs wspolnoty</t>
+  </si>
+  <si>
+    <t>granie w planszowki</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>lepszy pozadek w domu</t>
+  </si>
+  <si>
+    <t>czestsze jezdzenie na pszok</t>
+  </si>
+  <si>
+    <t>wymiana list przypodlogowych</t>
+  </si>
+  <si>
+    <t>pomalowanie calego domu</t>
+  </si>
+  <si>
+    <t>wymiana list progowych</t>
+  </si>
+  <si>
+    <t>zorganizowanie moich urodzin</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>wycieczka w tatry na weekend</t>
+  </si>
+  <si>
+    <t>wycieczka na weekend z dziecmi (dla dzieci)</t>
+  </si>
+  <si>
+    <t>swietowanie rocznicy slubu</t>
+  </si>
+  <si>
+    <t>wspolne wakacje</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>nie mieć pozyczek</t>
+  </si>
+  <si>
+    <t>przychody wieksze niż koszty</t>
+  </si>
+  <si>
+    <t>Raz w miesiacu gdzies wyjsc</t>
+  </si>
+  <si>
+    <t>Zaskakiwać</t>
+  </si>
+  <si>
+    <t>Stac się mniej dostepnym</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>historyjki/taski</t>
+  </si>
+  <si>
+    <t>Increase my confidance</t>
+  </si>
+  <si>
+    <t>overpay a loan 10k</t>
+  </si>
+  <si>
+    <t>FTP 270</t>
+  </si>
+  <si>
+    <t>winter swimming</t>
+  </si>
+  <si>
+    <t>attend to winter swimming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">well dressed; greate posture; have plan for future; </t>
+  </si>
+  <si>
+    <t>gain ftp 270 in test</t>
+  </si>
+  <si>
+    <t>powtarzalne</t>
+  </si>
+  <si>
+    <t>nie</t>
+  </si>
+  <si>
+    <t>tak</t>
+  </si>
+  <si>
+    <t>Pi Planing</t>
+  </si>
+  <si>
+    <t>Settelments:</t>
+  </si>
+  <si>
+    <t>Planowac 5 najblizszych sprintow</t>
+  </si>
+  <si>
+    <t>Reorganizowanie priorytetow</t>
+  </si>
+  <si>
+    <t>PI Scheduls:</t>
+  </si>
+  <si>
+    <t>PI1</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>Sprint 8</t>
+  </si>
+  <si>
+    <t>Sprint 9</t>
+  </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Sprint 11</t>
+  </si>
+  <si>
+    <t>Sprint 12</t>
+  </si>
+  <si>
+    <t>Sprint 13</t>
+  </si>
+  <si>
+    <t>PI3</t>
+  </si>
+  <si>
+    <t>Sprint 14</t>
+  </si>
+  <si>
+    <t>Sprint 15</t>
+  </si>
+  <si>
+    <t>Sprint 16</t>
+  </si>
+  <si>
+    <t>Sprint 17</t>
+  </si>
+  <si>
+    <t>Sprint 18</t>
+  </si>
+  <si>
+    <t>Sprint 19</t>
+  </si>
+  <si>
+    <t>Sprint 20</t>
+  </si>
+  <si>
+    <t>Sprint 21</t>
+  </si>
+  <si>
+    <t>Sprint 22</t>
+  </si>
+  <si>
+    <t>Sprint 23</t>
+  </si>
+  <si>
+    <t>Sprint 24</t>
+  </si>
+  <si>
+    <t>Sprint 25</t>
+  </si>
+  <si>
+    <t>Sprint 26</t>
+  </si>
+  <si>
+    <t>Sprint 27</t>
+  </si>
+  <si>
+    <t>PI4</t>
+  </si>
+  <si>
+    <t>Sprint 28</t>
+  </si>
+  <si>
+    <t>Sprint 29</t>
+  </si>
+  <si>
+    <t>PI5</t>
+  </si>
+  <si>
+    <t>PI2*</t>
+  </si>
+  <si>
+    <t>każdy Pi okres musi mieć storisy z kazdego epicu</t>
+  </si>
+  <si>
+    <t>Stories&gt;</t>
+  </si>
+  <si>
+    <t>Epics</t>
+  </si>
+  <si>
+    <t>E-bike (x)</t>
+  </si>
+  <si>
+    <t>Nose surgery (x)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMS(x) </t>
+  </si>
+  <si>
+    <t>Wedding Anniversary Celebration</t>
+  </si>
+  <si>
+    <t>x (4)</t>
+  </si>
+  <si>
+    <t>Go to PSZOK</t>
+  </si>
+  <si>
+    <t>x (5)</t>
+  </si>
+  <si>
+    <t>x (8)</t>
+  </si>
+  <si>
+    <t>x (6)</t>
+  </si>
+  <si>
+    <t>x (7)</t>
+  </si>
+  <si>
+    <t>Dbt Certification</t>
+  </si>
+  <si>
+    <t>Replacement Of Door Sills</t>
+  </si>
+  <si>
+    <t>Tomek's birthday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -508,11 +871,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCC4A04-F758-3449-AF3F-807EF5B35414}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="G37:H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56D75E4-527F-DC40-AF3F-9A185D23884B}">
-  <dimension ref="C9:N30"/>
+  <dimension ref="C1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="144" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,9 +898,16 @@
     <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>4</v>
@@ -660,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>8</v>
       </c>
@@ -668,7 +1052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>9</v>
       </c>
@@ -676,7 +1060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>10</v>
       </c>
@@ -684,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>11</v>
       </c>
@@ -692,7 +1076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>12</v>
       </c>
@@ -700,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>13</v>
       </c>
@@ -708,7 +1092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>14</v>
       </c>
@@ -716,38 +1100,503 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>28</v>
       </c>
       <c r="F27">
         <v>2025</v>
       </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
       <c r="H27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="N27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>29</v>
       </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
       <c r="H28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="K28" t="s">
+        <v>87</v>
+      </c>
+      <c r="L28" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" t="s">
+        <v>87</v>
+      </c>
+      <c r="L29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" t="s">
+        <v>51</v>
+      </c>
+      <c r="N29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>31</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" t="s">
+        <v>87</v>
+      </c>
+      <c r="L30" t="s">
+        <v>56</v>
+      </c>
+      <c r="M30" t="s">
+        <v>53</v>
+      </c>
+      <c r="N30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31" t="s">
+        <v>46</v>
+      </c>
+      <c r="K31" t="s">
+        <v>87</v>
+      </c>
+      <c r="L31" t="s">
+        <v>56</v>
+      </c>
+      <c r="M31" t="s">
+        <v>54</v>
+      </c>
+      <c r="N31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>7</v>
+      </c>
+      <c r="H32" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" t="s">
+        <v>87</v>
+      </c>
+      <c r="L32" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" t="s">
+        <v>87</v>
+      </c>
+      <c r="L33" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" t="s">
+        <v>57</v>
+      </c>
+      <c r="N33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" t="s">
+        <v>87</v>
+      </c>
+      <c r="L34" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" t="s">
+        <v>59</v>
+      </c>
+      <c r="N34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="K35" t="s">
+        <v>87</v>
+      </c>
+      <c r="L35" t="s">
+        <v>58</v>
+      </c>
+      <c r="M35" t="s">
+        <v>60</v>
+      </c>
+      <c r="N35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>11</v>
+      </c>
+      <c r="K36" t="s">
+        <v>87</v>
+      </c>
+      <c r="L36" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" t="s">
+        <v>61</v>
+      </c>
+      <c r="N36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>87</v>
+      </c>
+      <c r="L37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M37" t="s">
+        <v>62</v>
+      </c>
+      <c r="N37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K38" t="s">
+        <v>87</v>
+      </c>
+      <c r="L38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M38" t="s">
+        <v>63</v>
+      </c>
+      <c r="N38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K39" t="s">
+        <v>87</v>
+      </c>
+      <c r="L39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M39" t="s">
+        <v>64</v>
+      </c>
+      <c r="N39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K40" t="s">
+        <v>87</v>
+      </c>
+      <c r="L40" t="s">
+        <v>65</v>
+      </c>
+      <c r="M40" t="s">
+        <v>66</v>
+      </c>
+      <c r="N40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K41" t="s">
+        <v>87</v>
+      </c>
+      <c r="L41" t="s">
+        <v>65</v>
+      </c>
+      <c r="M41" t="s">
+        <v>67</v>
+      </c>
+      <c r="N41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K42" t="s">
+        <v>87</v>
+      </c>
+      <c r="L42" t="s">
+        <v>65</v>
+      </c>
+      <c r="M42" t="s">
+        <v>68</v>
+      </c>
+      <c r="N42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K43" t="s">
+        <v>87</v>
+      </c>
+      <c r="L43" t="s">
+        <v>65</v>
+      </c>
+      <c r="M43" t="s">
+        <v>75</v>
+      </c>
+      <c r="N43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K44" t="s">
+        <v>88</v>
+      </c>
+      <c r="L44" t="s">
+        <v>69</v>
+      </c>
+      <c r="M44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K45" t="s">
+        <v>88</v>
+      </c>
+      <c r="L45" t="s">
+        <v>69</v>
+      </c>
+      <c r="M45" t="s">
+        <v>71</v>
+      </c>
+      <c r="N45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K46" t="s">
+        <v>88</v>
+      </c>
+      <c r="L46" t="s">
+        <v>69</v>
+      </c>
+      <c r="M46" t="s">
+        <v>72</v>
+      </c>
+      <c r="N46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K47" t="s">
+        <v>88</v>
+      </c>
+      <c r="L47" t="s">
+        <v>69</v>
+      </c>
+      <c r="M47" t="s">
+        <v>73</v>
+      </c>
+      <c r="N47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="K48" t="s">
+        <v>88</v>
+      </c>
+      <c r="L48" t="s">
+        <v>69</v>
+      </c>
+      <c r="M48" t="s">
+        <v>74</v>
+      </c>
+      <c r="N48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K49" t="s">
+        <v>88</v>
+      </c>
+      <c r="L49" t="s">
+        <v>76</v>
+      </c>
+      <c r="M49" t="s">
+        <v>77</v>
+      </c>
+      <c r="N49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K50" t="s">
+        <v>88</v>
+      </c>
+      <c r="L50" t="s">
+        <v>76</v>
+      </c>
+      <c r="M50" t="s">
+        <v>78</v>
+      </c>
+      <c r="N50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K51" t="s">
+        <v>88</v>
+      </c>
+      <c r="L51" t="s">
+        <v>76</v>
+      </c>
+      <c r="M51" t="s">
+        <v>79</v>
+      </c>
+      <c r="N51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K52" t="s">
+        <v>88</v>
+      </c>
+      <c r="L52" t="s">
+        <v>76</v>
+      </c>
+      <c r="M52" t="s">
+        <v>80</v>
+      </c>
+      <c r="N52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K53" t="s">
+        <v>88</v>
+      </c>
+      <c r="L53" t="s">
+        <v>76</v>
+      </c>
+      <c r="M53" t="s">
+        <v>84</v>
+      </c>
+      <c r="N53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K54" t="s">
+        <v>88</v>
+      </c>
+      <c r="L54" t="s">
+        <v>76</v>
+      </c>
+      <c r="M54" t="s">
+        <v>85</v>
+      </c>
+      <c r="N54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K55" t="s">
+        <v>88</v>
+      </c>
+      <c r="L55" t="s">
+        <v>76</v>
+      </c>
+      <c r="M55" t="s">
+        <v>86</v>
+      </c>
+      <c r="N55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K60" t="s">
+        <v>88</v>
+      </c>
+      <c r="L60" t="s">
+        <v>81</v>
+      </c>
+      <c r="M60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="K61" t="s">
+        <v>88</v>
+      </c>
+      <c r="L61" t="s">
+        <v>81</v>
+      </c>
+      <c r="M61" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -756,4 +1605,418 @@
     <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K0000FF TechnipFMC | Internal&amp;1#_x000D_</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E3B492-324E-164C-BCA1-C4C699410355}">
+  <dimension ref="H8:R21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="8:18" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="8:18" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="8:18" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="8:18" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17">
+        <v>2024</v>
+      </c>
+      <c r="L17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>90</v>
+      </c>
+      <c r="L19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>91</v>
+      </c>
+      <c r="L20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0F8EE0-4B3A-2E49-92B1-FFC547BAFD69}">
+  <dimension ref="B6:O34"/>
+  <sheetViews>
+    <sheetView zoomScale="141" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" t="s">
+        <v>142</v>
+      </c>
+      <c r="L7" t="s">
+        <v>144</v>
+      </c>
+      <c r="M7" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" t="s">
+        <v>149</v>
+      </c>
+      <c r="O7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" t="s">
+        <v>143</v>
+      </c>
+      <c r="J9" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" t="s">
+        <v>145</v>
+      </c>
+      <c r="J10" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>147</v>
+      </c>
+      <c r="M11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" t="s">
+        <v>148</v>
+      </c>
+      <c r="N12" t="s">
+        <v>148</v>
+      </c>
+      <c r="O12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J13" t="s">
+        <v>146</v>
+      </c>
+      <c r="L13" t="s">
+        <v>146</v>
+      </c>
+      <c r="N13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new task from add activity page
</commit_message>
<xml_diff>
--- a/data/2025_goals.xlsx
+++ b/data/2025_goals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tferenc/ebis/task_management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449ACB7A-697E-204D-9C2E-4EEA87153DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAD6938-F2C8-1040-B5DA-B5A6663CB038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38380" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
+    <workbookView xWindow="38420" yWindow="500" windowWidth="38400" windowHeight="19260" activeTab="3" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaulation 2024" sheetId="2" r:id="rId1"/>
@@ -38,8 +38,71 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={ED0FF008-645C-E844-B260-A10CD3997D23}</author>
+    <author>tc={8096D727-C8BD-D84B-861A-2E850DF54541}</author>
+    <author>tc={5097C933-87B2-E04E-96C3-24B5C0CB2D82}</author>
+    <author>tc={03BCF80E-9AE7-5F45-88AA-23A55BDADE3D}</author>
+    <author>tc={B6084FDF-73E2-BF4D-84CB-BC9E065D3962}</author>
+  </authors>
+  <commentList>
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{ED0FF008-645C-E844-B260-A10CD3997D23}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Prepare and go</t>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="1" shapeId="0" xr:uid="{8096D727-C8BD-D84B-861A-2E850DF54541}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1. Figure out what to do
+2. Find out who can look after our kinds
+3. Prepare everything
+4. Make it</t>
+      </text>
+    </comment>
+    <comment ref="D24" authorId="2" shapeId="0" xr:uid="{5097C933-87B2-E04E-96C3-24B5C0CB2D82}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1. Go to castorama and buy
+2. Remove Old One
+3. Instal New One</t>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="3" shapeId="0" xr:uid="{03BCF80E-9AE7-5F45-88AA-23A55BDADE3D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1. Maka a decision of making it
+2. Prepare a list of guests
+3. Invite everyone
+4. Make a party</t>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="4" shapeId="0" xr:uid="{B6084FDF-73E2-BF4D-84CB-BC9E065D3962}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1 Plan
+2. Make it</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="179">
   <si>
     <t>dbt</t>
   </si>
@@ -254,9 +317,6 @@
     <t>lepszy pozadek w domu</t>
   </si>
   <si>
-    <t>czestsze jezdzenie na pszok</t>
-  </si>
-  <si>
     <t>wymiana list przypodlogowych</t>
   </si>
   <si>
@@ -266,9 +326,6 @@
     <t>wymiana list progowych</t>
   </si>
   <si>
-    <t>zorganizowanie moich urodzin</t>
-  </si>
-  <si>
     <t>Family</t>
   </si>
   <si>
@@ -278,9 +335,6 @@
     <t>wycieczka na weekend z dziecmi (dla dzieci)</t>
   </si>
   <si>
-    <t>swietowanie rocznicy slubu</t>
-  </si>
-  <si>
     <t>wspolne wakacje</t>
   </si>
   <si>
@@ -293,9 +347,6 @@
     <t>przychody wieksze niż koszty</t>
   </si>
   <si>
-    <t>Raz w miesiacu gdzies wyjsc</t>
-  </si>
-  <si>
     <t>Zaskakiwać</t>
   </si>
   <si>
@@ -470,24 +521,9 @@
     <t>Wedding Anniversary Celebration</t>
   </si>
   <si>
-    <t>x (4)</t>
-  </si>
-  <si>
     <t>Go to PSZOK</t>
   </si>
   <si>
-    <t>x (5)</t>
-  </si>
-  <si>
-    <t>x (8)</t>
-  </si>
-  <si>
-    <t>x (6)</t>
-  </si>
-  <si>
-    <t>x (7)</t>
-  </si>
-  <si>
     <t>Dbt Certification</t>
   </si>
   <si>
@@ -495,6 +531,114 @@
   </si>
   <si>
     <t>Tomek's birthday</t>
+  </si>
+  <si>
+    <t>4 tasks</t>
+  </si>
+  <si>
+    <t>2 tasks</t>
+  </si>
+  <si>
+    <t>1 task</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>half a day</t>
+  </si>
+  <si>
+    <t>whole day</t>
+  </si>
+  <si>
+    <t>couple of days</t>
+  </si>
+  <si>
+    <t>3 tasks</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Go outside</t>
+  </si>
+  <si>
+    <t>Time Without Wife</t>
+  </si>
+  <si>
+    <t>30 per sprint</t>
+  </si>
+  <si>
+    <t>Go Outside</t>
+  </si>
+  <si>
+    <t>sprzatanie strychu</t>
+  </si>
+  <si>
+    <t>sprzatanie komorki lokatorskiej</t>
+  </si>
+  <si>
+    <t>sprzatanie samochodu</t>
+  </si>
+  <si>
+    <t>Czytac ksiazki</t>
+  </si>
+  <si>
+    <t>wziąć dzieci na meska wyprawe</t>
+  </si>
+  <si>
+    <t>wziąć dzieci na meska wyprawe z noclegiem</t>
+  </si>
+  <si>
+    <t>wziąć dzieci na basen</t>
+  </si>
+  <si>
+    <t>spowiedź raz na PI</t>
+  </si>
+  <si>
+    <t>Life Rules</t>
+  </si>
+  <si>
+    <t>Wychowuje zdrowe, zaradne dzieci dla których jestem wzorem</t>
+  </si>
+  <si>
+    <t>Jestem dobrym, skutecznym i pewnym siebie mezczyzna</t>
+  </si>
+  <si>
+    <t>Jezus jest moja osobista sila</t>
+  </si>
+  <si>
+    <t>Main goals</t>
+  </si>
+  <si>
+    <t>Go to Confession</t>
+  </si>
+  <si>
+    <t>Dbam o rodzine</t>
+  </si>
+  <si>
+    <t>zabrac dzieci do kina</t>
+  </si>
+  <si>
+    <t>Spac z dziecmi pod namiotem</t>
+  </si>
+  <si>
+    <t>Read Book</t>
+  </si>
+  <si>
+    <t>Added to app</t>
+  </si>
+  <si>
+    <t>Go to PSZOK (x)</t>
+  </si>
+  <si>
+    <t>Take Kids to the Cinema</t>
+  </si>
+  <si>
+    <t>Python - task management</t>
   </si>
 </sst>
 </file>
@@ -516,12 +660,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -536,8 +692,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,6 +711,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Tomasz Ferenc" id="{33553C0B-BB3C-374C-BF53-4C47DA1868FB}" userId="S::tomasz.ferenc@technipfmc.com::a93253ce-5a00-4255-a81d-9ddbc264febc" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -870,6 +1034,35 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D21" dT="2024-12-11T09:54:32.22" personId="{33553C0B-BB3C-374C-BF53-4C47DA1868FB}" id="{ED0FF008-645C-E844-B260-A10CD3997D23}">
+    <text>Prepare and go</text>
+  </threadedComment>
+  <threadedComment ref="D23" dT="2024-12-11T09:58:11.06" personId="{33553C0B-BB3C-374C-BF53-4C47DA1868FB}" id="{8096D727-C8BD-D84B-861A-2E850DF54541}">
+    <text>1. Figure out what to do
+2. Find out who can look after our kinds
+3. Prepare everything
+4. Make it</text>
+  </threadedComment>
+  <threadedComment ref="D24" dT="2024-12-11T09:59:57.12" personId="{33553C0B-BB3C-374C-BF53-4C47DA1868FB}" id="{5097C933-87B2-E04E-96C3-24B5C0CB2D82}">
+    <text>1. Go to castorama and buy
+2. Remove Old One
+3. Instal New One</text>
+  </threadedComment>
+  <threadedComment ref="D25" dT="2024-12-11T10:08:00.63" personId="{33553C0B-BB3C-374C-BF53-4C47DA1868FB}" id="{03BCF80E-9AE7-5F45-88AA-23A55BDADE3D}">
+    <text>1. Maka a decision of making it
+2. Prepare a list of guests
+3. Invite everyone
+4. Make a party</text>
+  </threadedComment>
+  <threadedComment ref="D27" dT="2024-12-11T10:52:20.43" personId="{33553C0B-BB3C-374C-BF53-4C47DA1868FB}" id="{B6084FDF-73E2-BF4D-84CB-BC9E065D3962}">
+    <text>1 Plan
+2. Make it</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCC4A04-F758-3449-AF3F-807EF5B35414}">
   <dimension ref="A1"/>
@@ -886,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56D75E4-527F-DC40-AF3F-9A185D23884B}">
-  <dimension ref="C1:N61"/>
+  <dimension ref="C1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="144" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="D1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,7 +1098,7 @@
   <sheetData>
     <row r="1" spans="4:14" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.2">
@@ -1108,7 +1301,7 @@
         <v>33</v>
       </c>
       <c r="M26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
@@ -1125,7 +1318,7 @@
         <v>32</v>
       </c>
       <c r="N27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.2">
@@ -1139,7 +1332,7 @@
         <v>49</v>
       </c>
       <c r="K28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L28" t="s">
         <v>56</v>
@@ -1148,7 +1341,7 @@
         <v>52</v>
       </c>
       <c r="N28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
@@ -1162,7 +1355,7 @@
         <v>34</v>
       </c>
       <c r="K29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L29" t="s">
         <v>56</v>
@@ -1171,7 +1364,7 @@
         <v>51</v>
       </c>
       <c r="N29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.2">
@@ -1185,7 +1378,7 @@
         <v>45</v>
       </c>
       <c r="K30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L30" t="s">
         <v>56</v>
@@ -1194,7 +1387,7 @@
         <v>53</v>
       </c>
       <c r="N30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.2">
@@ -1205,7 +1398,7 @@
         <v>46</v>
       </c>
       <c r="K31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L31" t="s">
         <v>56</v>
@@ -1214,7 +1407,7 @@
         <v>54</v>
       </c>
       <c r="N31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.2">
@@ -1225,7 +1418,7 @@
         <v>47</v>
       </c>
       <c r="K32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L32" t="s">
         <v>56</v>
@@ -1234,7 +1427,7 @@
         <v>55</v>
       </c>
       <c r="N32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="7:14" x14ac:dyDescent="0.2">
@@ -1245,7 +1438,7 @@
         <v>48</v>
       </c>
       <c r="K33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L33" t="s">
         <v>56</v>
@@ -1254,7 +1447,7 @@
         <v>57</v>
       </c>
       <c r="N33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="7:14" x14ac:dyDescent="0.2">
@@ -1265,7 +1458,7 @@
         <v>50</v>
       </c>
       <c r="K34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L34" t="s">
         <v>58</v>
@@ -1274,7 +1467,7 @@
         <v>59</v>
       </c>
       <c r="N34" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="7:14" x14ac:dyDescent="0.2">
@@ -1282,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="K35" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L35" t="s">
         <v>58</v>
@@ -1291,7 +1484,7 @@
         <v>60</v>
       </c>
       <c r="N35" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="7:14" x14ac:dyDescent="0.2">
@@ -1299,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="K36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L36" t="s">
         <v>58</v>
@@ -1308,12 +1501,12 @@
         <v>61</v>
       </c>
       <c r="N36" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L37" t="s">
         <v>58</v>
@@ -1322,12 +1515,12 @@
         <v>62</v>
       </c>
       <c r="N37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L38" t="s">
         <v>58</v>
@@ -1336,12 +1529,12 @@
         <v>63</v>
       </c>
       <c r="N38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L39" t="s">
         <v>58</v>
@@ -1350,12 +1543,12 @@
         <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L40" t="s">
         <v>65</v>
@@ -1364,12 +1557,12 @@
         <v>66</v>
       </c>
       <c r="N40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L41" t="s">
         <v>65</v>
@@ -1378,12 +1571,12 @@
         <v>67</v>
       </c>
       <c r="N41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L42" t="s">
         <v>65</v>
@@ -1392,26 +1585,17 @@
         <v>68</v>
       </c>
       <c r="N42" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K43" t="s">
-        <v>87</v>
-      </c>
-      <c r="L43" t="s">
-        <v>65</v>
-      </c>
-      <c r="M43" t="s">
-        <v>75</v>
-      </c>
-      <c r="N43" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L44" t="s">
         <v>69</v>
@@ -1420,183 +1604,252 @@
         <v>70</v>
       </c>
       <c r="N44" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K45" t="s">
-        <v>88</v>
-      </c>
-      <c r="L45" t="s">
-        <v>69</v>
-      </c>
-      <c r="M45" t="s">
-        <v>71</v>
-      </c>
-      <c r="N45" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L46" t="s">
         <v>69</v>
       </c>
       <c r="M46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N46" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K47" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L47" t="s">
         <v>69</v>
       </c>
       <c r="M47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="7:14" x14ac:dyDescent="0.2">
       <c r="K48" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L48" t="s">
         <v>69</v>
       </c>
       <c r="M48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N48" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M49" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N49" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K50" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L50" t="s">
+        <v>74</v>
+      </c>
+      <c r="M50" t="s">
         <v>76</v>
       </c>
-      <c r="M50" t="s">
-        <v>78</v>
-      </c>
       <c r="N50" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K51" t="s">
-        <v>88</v>
-      </c>
-      <c r="L51" t="s">
-        <v>76</v>
-      </c>
-      <c r="M51" t="s">
-        <v>79</v>
-      </c>
-      <c r="N51" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K52" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M52" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N52" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K53" t="s">
-        <v>88</v>
-      </c>
-      <c r="L53" t="s">
-        <v>76</v>
-      </c>
-      <c r="M53" t="s">
         <v>84</v>
-      </c>
-      <c r="N53" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="54" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K54" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M54" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N54" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K55" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L55" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M55" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N55" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K60" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K61" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L61" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M61" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="L62" t="s">
+        <v>69</v>
+      </c>
+      <c r="M62" t="s">
+        <v>157</v>
+      </c>
+      <c r="N62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="L63" t="s">
+        <v>69</v>
+      </c>
+      <c r="M63" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="11:14" x14ac:dyDescent="0.2">
+      <c r="L64" t="s">
+        <v>69</v>
+      </c>
+      <c r="M64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L65" t="s">
+        <v>58</v>
+      </c>
+      <c r="M65" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L66" t="s">
+        <v>65</v>
+      </c>
+      <c r="M66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L67" t="s">
+        <v>74</v>
+      </c>
+      <c r="M67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L68" t="s">
+        <v>74</v>
+      </c>
+      <c r="M68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L69" t="s">
+        <v>74</v>
+      </c>
+      <c r="M69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L70" t="s">
+        <v>56</v>
+      </c>
+      <c r="M70" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L71" t="s">
+        <v>74</v>
+      </c>
+      <c r="M71" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L72" t="s">
+        <v>74</v>
+      </c>
+      <c r="M72" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L73" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1609,10 +1862,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E3B492-324E-164C-BCA1-C4C699410355}">
-  <dimension ref="H8:R21"/>
+  <dimension ref="B8:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1621,22 +1874,47 @@
     <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="R8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="R9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>167</v>
+      </c>
       <c r="H15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>171</v>
+      </c>
       <c r="H16" t="s">
         <v>36</v>
       </c>
@@ -1653,21 +1931,27 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>168</v>
+      </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J17">
         <v>2024</v>
       </c>
       <c r="L17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H18">
         <v>2</v>
       </c>
@@ -1678,37 +1962,37 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H19">
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H20">
         <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H21">
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="L21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1717,27 +2001,75 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0F8EE0-4B3A-2E49-92B1-FFC547BAFD69}">
-  <dimension ref="B6:O34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0F8EE0-4B3A-2E49-92B1-FFC547BAFD69}">
+  <dimension ref="A2:V34"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:O13"/>
+    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G6" t="s">
-        <v>138</v>
-      </c>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="I2" s="2"/>
+      <c r="J2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H6" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="I6" t="s">
         <v>56</v>
@@ -1746,277 +2078,488 @@
         <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="M6" t="s">
         <v>69</v>
       </c>
       <c r="N6" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" t="s">
         <v>58</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" t="s">
+        <v>74</v>
+      </c>
+      <c r="U6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" t="s">
         <v>137</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K7" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" t="s">
         <v>141</v>
       </c>
-      <c r="I7" t="s">
+      <c r="O7" t="s">
         <v>140</v>
       </c>
-      <c r="J7" t="s">
-        <v>139</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="P7" t="s">
         <v>142</v>
       </c>
-      <c r="L7" t="s">
-        <v>144</v>
-      </c>
-      <c r="M7" t="s">
-        <v>150</v>
-      </c>
-      <c r="N7" t="s">
-        <v>149</v>
-      </c>
-      <c r="O7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>156</v>
+      </c>
+      <c r="R7" t="s">
+        <v>154</v>
+      </c>
+      <c r="S7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T7" t="s">
+        <v>177</v>
+      </c>
+      <c r="U7" t="s">
+        <v>174</v>
+      </c>
+      <c r="V7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8"/>
       <c r="B8" t="s">
-        <v>101</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
       <c r="F8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9">
+        <f>SUM(I9:XFD9)</f>
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
         <v>102</v>
       </c>
-      <c r="F9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>5</v>
+      </c>
+      <c r="L9" s="2">
+        <v>13</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3</v>
+      </c>
+      <c r="V9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G13" si="0">SUM(I10:XFD10)</f>
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
         <v>103</v>
       </c>
-      <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>145</v>
-      </c>
-      <c r="J10" t="s">
-        <v>145</v>
-      </c>
-      <c r="L10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+      <c r="R10" s="2">
+        <v>13</v>
+      </c>
+      <c r="U10" s="2">
+        <v>8</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>8</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>3</v>
+      </c>
+      <c r="T11" s="2">
+        <v>5</v>
+      </c>
+      <c r="V11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>13</v>
+      </c>
+      <c r="P12" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>5</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+      <c r="O13" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>3</v>
+      </c>
+      <c r="S13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>136</v>
       </c>
-      <c r="G11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H11" t="s">
-        <v>147</v>
-      </c>
-      <c r="J11" t="s">
-        <v>147</v>
-      </c>
-      <c r="M11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" t="s">
-        <v>148</v>
-      </c>
-      <c r="J12" t="s">
-        <v>148</v>
-      </c>
-      <c r="N12" t="s">
-        <v>148</v>
-      </c>
-      <c r="O12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G13" t="s">
-        <v>110</v>
-      </c>
-      <c r="H13" t="s">
-        <v>146</v>
-      </c>
-      <c r="J13" t="s">
-        <v>146</v>
-      </c>
-      <c r="L13" t="s">
-        <v>146</v>
-      </c>
-      <c r="N13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="F14" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G19" t="s">
+      <c r="D22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G20" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G21" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+      <c r="H25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G22" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G23" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G24" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F25" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>130</v>
+      </c>
+      <c r="H30" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G28" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F30" t="s">
-        <v>134</v>
-      </c>
-      <c r="G30" t="s">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G31" t="s">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G34" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add estimate date for tasks as a property
</commit_message>
<xml_diff>
--- a/data/2025_goals.xlsx
+++ b/data/2025_goals.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tferenc/ebis/task_management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAD6938-F2C8-1040-B5DA-B5A6663CB038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E000A66-0F3E-7E44-98B0-CBF112E493D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="500" windowWidth="38400" windowHeight="19260" activeTab="3" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="38400" windowHeight="19260" activeTab="5" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaulation 2024" sheetId="2" r:id="rId1"/>
     <sheet name="goals 2025" sheetId="1" r:id="rId2"/>
     <sheet name="Objectives" sheetId="3" r:id="rId3"/>
     <sheet name="PI planning" sheetId="4" r:id="rId4"/>
+    <sheet name="TM Review" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="205">
   <si>
     <t>dbt</t>
   </si>
@@ -639,6 +641,84 @@
   </si>
   <si>
     <t>Python - task management</t>
+  </si>
+  <si>
+    <t>Task management Review</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Everything Is ok</t>
+  </si>
+  <si>
+    <t>Add activity</t>
+  </si>
+  <si>
+    <t>put filters in frame</t>
+  </si>
+  <si>
+    <t>try colapse all stories as default view</t>
+  </si>
+  <si>
+    <t>Select sprint shows only sprint from PI</t>
+  </si>
+  <si>
+    <t>Add PI dropdown with all option</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>select epic add all option as default</t>
+  </si>
+  <si>
+    <t>Add ability to create story and assign to backlog</t>
+  </si>
+  <si>
+    <t>add filter with current sprint and current pi</t>
+  </si>
+  <si>
+    <t>add ability to change epic for story</t>
+  </si>
+  <si>
+    <t>add to story allighment to Objectives</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Add execution estimate date to tasks</t>
+  </si>
+  <si>
+    <t>Create simple  notiffication email (using python anywhere)</t>
+  </si>
+  <si>
+    <t>plan glowny</t>
+  </si>
+  <si>
+    <t>wyjscie na pilsko</t>
+  </si>
+  <si>
+    <t>prezet</t>
+  </si>
+  <si>
+    <t>kolacja w piątek</t>
+  </si>
+  <si>
+    <t>w razie nie pogody</t>
+  </si>
+  <si>
+    <t>lodowisko</t>
+  </si>
+  <si>
+    <t>śniadanie</t>
+  </si>
+  <si>
+    <t>kino</t>
+  </si>
+  <si>
+    <t>obiad</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1148,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="G37:H37"/>
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56D75E4-527F-DC40-AF3F-9A185D23884B}">
   <dimension ref="C1:N73"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView topLeftCell="E1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1865,7 +1945,7 @@
   <dimension ref="B8:R21"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G21" sqref="A21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2004,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0F8EE0-4B3A-2E49-92B1-FFC547BAFD69}">
   <dimension ref="A2:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="O54" sqref="C53:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2562,4 +2642,164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE59998-FE14-BB41-8DAC-846E2751A945}">
+  <dimension ref="D5:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF650962-3039-C946-B719-F50AF22BC3A0}">
+  <dimension ref="F12:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix issues related to estimate date for tasks
</commit_message>
<xml_diff>
--- a/data/2025_goals.xlsx
+++ b/data/2025_goals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tferenc/ebis/task_management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E000A66-0F3E-7E44-98B0-CBF112E493D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802CDFF2-5469-3F49-895A-7CB15860152D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="38400" windowHeight="19260" activeTab="5" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="34560" windowHeight="19260" activeTab="6" xr2:uid="{49CE68EC-A879-6946-98CF-558F0C488244}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaulation 2024" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Objectives" sheetId="3" r:id="rId3"/>
     <sheet name="PI planning" sheetId="4" r:id="rId4"/>
     <sheet name="TM Review" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="R" sheetId="6" r:id="rId6"/>
+    <sheet name="F" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="208">
   <si>
     <t>dbt</t>
   </si>
@@ -719,6 +720,15 @@
   </si>
   <si>
     <t>obiad</t>
+  </si>
+  <si>
+    <t>tomek</t>
+  </si>
+  <si>
+    <t>marzenka</t>
+  </si>
+  <si>
+    <t>800+</t>
   </si>
 </sst>
 </file>
@@ -2744,7 +2754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF650962-3039-C946-B719-F50AF22BC3A0}">
   <dimension ref="F12:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
@@ -2802,4 +2812,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A631A2-B521-B04C-B641-75DE2F599358}">
+  <dimension ref="L13:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="13" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>205</v>
+      </c>
+      <c r="M13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>206</v>
+      </c>
+      <c r="M14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>207</v>
+      </c>
+      <c r="M15">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="16" spans="12:15" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <f>SUM(M13:M15)</f>
+        <v>6600</v>
+      </c>
+      <c r="O16">
+        <f>M16*12</f>
+        <v>79200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>